<commit_message>
be strict with myself
</commit_message>
<xml_diff>
--- a/first.xlsx
+++ b/first.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26215"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Workspace/DongSongtao/workspace/dream_plan/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13060"/>
+    <workbookView windowWidth="28695" windowHeight="13050"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,16 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14">
   <si>
     <t>Time/effective</t>
   </si>
@@ -73,8 +63,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,13 +79,151 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -98,7 +232,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -122,24 +256,210 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -162,9 +482,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -196,32 +758,79 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -512,28 +1121,28 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:P74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6666666666667" style="1" customWidth="1"/>
     <col min="2" max="4" width="9" style="1"/>
-    <col min="5" max="5" width="11.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1666666666667" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1666666666667" style="1" customWidth="1"/>
     <col min="7" max="8" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="37" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" ht="37" customHeight="1" spans="1:16">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -558,14 +1167,14 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="14"/>
-    </row>
-    <row r="2" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K1" s="10"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="15"/>
+    </row>
+    <row r="2" ht="20" customHeight="1" spans="1:16">
       <c r="A2" s="4">
         <v>43119</v>
       </c>
@@ -594,21 +1203,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" ht="20" customHeight="1" spans="1:8">
       <c r="A3" s="4">
         <v>43120</v>
       </c>
       <c r="B3" s="5"/>
-      <c r="C3" s="15"/>
+      <c r="C3" s="9"/>
       <c r="D3" s="5"/>
-      <c r="E3" s="15"/>
+      <c r="E3" s="9"/>
       <c r="F3" s="7"/>
       <c r="G3" s="8">
         <v>75</v>
       </c>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" ht="20" customHeight="1" spans="1:8">
       <c r="A4" s="4">
         <v>43121</v>
       </c>
@@ -622,31 +1231,31 @@
       </c>
       <c r="H4" s="8"/>
     </row>
-    <row r="5" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" ht="20" customHeight="1" spans="1:8">
       <c r="A5" s="4">
         <v>43122</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="5"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" ht="20" customHeight="1" spans="1:8">
       <c r="A6" s="4">
         <v>43123</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="7"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" ht="20" customHeight="1" spans="1:8">
       <c r="A7" s="4">
         <v>43124</v>
       </c>
@@ -658,7 +1267,7 @@
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
     </row>
-    <row r="8" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" ht="20" customHeight="1" spans="1:8">
       <c r="A8" s="4">
         <v>43125</v>
       </c>
@@ -670,7 +1279,7 @@
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
     </row>
-    <row r="9" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" ht="20" customHeight="1" spans="1:8">
       <c r="A9" s="4">
         <v>43126</v>
       </c>
@@ -682,7 +1291,7 @@
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
     </row>
-    <row r="10" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" ht="20" customHeight="1" spans="1:8">
       <c r="A10" s="4">
         <v>43127</v>
       </c>
@@ -694,7 +1303,7 @@
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
     </row>
-    <row r="11" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" ht="20" customHeight="1" spans="1:8">
       <c r="A11" s="4">
         <v>43128</v>
       </c>
@@ -706,7 +1315,7 @@
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
     </row>
-    <row r="12" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" ht="20" customHeight="1" spans="1:8">
       <c r="A12" s="4">
         <v>43129</v>
       </c>
@@ -718,7 +1327,7 @@
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
     </row>
-    <row r="13" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" ht="20" customHeight="1" spans="1:8">
       <c r="A13" s="4">
         <v>43130</v>
       </c>
@@ -730,7 +1339,7 @@
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
     </row>
-    <row r="14" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" ht="20" customHeight="1" spans="1:8">
       <c r="A14" s="4">
         <v>43131</v>
       </c>
@@ -742,7 +1351,7 @@
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
     </row>
-    <row r="15" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" ht="20" customHeight="1" spans="1:8">
       <c r="A15" s="4">
         <v>43132</v>
       </c>
@@ -754,7 +1363,7 @@
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
     </row>
-    <row r="16" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" ht="20" customHeight="1" spans="1:8">
       <c r="A16" s="4">
         <v>43133</v>
       </c>
@@ -766,7 +1375,7 @@
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
     </row>
-    <row r="17" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" ht="20" customHeight="1" spans="1:8">
       <c r="A17" s="4">
         <v>43134</v>
       </c>
@@ -778,7 +1387,7 @@
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
     </row>
-    <row r="18" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" ht="20" customHeight="1" spans="1:8">
       <c r="A18" s="4">
         <v>43135</v>
       </c>
@@ -790,7 +1399,7 @@
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
     </row>
-    <row r="19" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" ht="20" customHeight="1" spans="1:8">
       <c r="A19" s="4">
         <v>43136</v>
       </c>
@@ -802,7 +1411,7 @@
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
     </row>
-    <row r="20" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" ht="20" customHeight="1" spans="1:8">
       <c r="A20" s="4">
         <v>43137</v>
       </c>
@@ -814,7 +1423,7 @@
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
     </row>
-    <row r="21" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" ht="20" customHeight="1" spans="1:8">
       <c r="A21" s="4">
         <v>43138</v>
       </c>
@@ -826,7 +1435,7 @@
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
     </row>
-    <row r="22" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" ht="20" customHeight="1" spans="1:8">
       <c r="A22" s="4">
         <v>43139</v>
       </c>
@@ -838,7 +1447,7 @@
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
     </row>
-    <row r="23" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" ht="20" customHeight="1" spans="1:8">
       <c r="A23" s="4">
         <v>43140</v>
       </c>
@@ -850,7 +1459,7 @@
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
     </row>
-    <row r="24" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" ht="20" customHeight="1" spans="1:8">
       <c r="A24" s="4">
         <v>43141</v>
       </c>
@@ -862,7 +1471,7 @@
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
     </row>
-    <row r="25" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" ht="20" customHeight="1" spans="1:8">
       <c r="A25" s="4">
         <v>43142</v>
       </c>
@@ -874,7 +1483,7 @@
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
     </row>
-    <row r="26" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" ht="20" customHeight="1" spans="1:8">
       <c r="A26" s="4">
         <v>43143</v>
       </c>
@@ -886,7 +1495,7 @@
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
     </row>
-    <row r="27" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" ht="20" customHeight="1" spans="1:8">
       <c r="A27" s="4">
         <v>43144</v>
       </c>
@@ -898,7 +1507,7 @@
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
     </row>
-    <row r="28" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" ht="20" customHeight="1" spans="1:8">
       <c r="A28" s="4">
         <v>43145</v>
       </c>
@@ -910,7 +1519,7 @@
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
     </row>
-    <row r="29" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" ht="20" customHeight="1" spans="1:8">
       <c r="A29" s="4">
         <v>43146</v>
       </c>
@@ -922,7 +1531,7 @@
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
     </row>
-    <row r="30" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" ht="20" customHeight="1" spans="1:8">
       <c r="A30" s="4">
         <v>43147</v>
       </c>
@@ -934,7 +1543,7 @@
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
     </row>
-    <row r="31" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" ht="20" customHeight="1" spans="1:8">
       <c r="A31" s="4">
         <v>43148</v>
       </c>
@@ -946,7 +1555,7 @@
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
     </row>
-    <row r="32" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" ht="20" customHeight="1" spans="1:8">
       <c r="A32" s="4">
         <v>43149</v>
       </c>
@@ -958,7 +1567,7 @@
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
     </row>
-    <row r="33" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" ht="20" customHeight="1" spans="1:8">
       <c r="A33" s="4">
         <v>43150</v>
       </c>
@@ -970,7 +1579,7 @@
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
     </row>
-    <row r="34" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" ht="20" customHeight="1" spans="1:8">
       <c r="A34" s="4">
         <v>43151</v>
       </c>
@@ -982,7 +1591,7 @@
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
     </row>
-    <row r="35" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" ht="20" customHeight="1" spans="1:8">
       <c r="A35" s="4">
         <v>43152</v>
       </c>
@@ -994,7 +1603,7 @@
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>
     </row>
-    <row r="36" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" ht="20" customHeight="1" spans="1:8">
       <c r="A36" s="4">
         <v>43153</v>
       </c>
@@ -1006,7 +1615,7 @@
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
     </row>
-    <row r="37" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" ht="20" customHeight="1" spans="1:8">
       <c r="A37" s="4">
         <v>43154</v>
       </c>
@@ -1018,7 +1627,7 @@
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
     </row>
-    <row r="38" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" ht="20" customHeight="1" spans="1:8">
       <c r="A38" s="4">
         <v>43155</v>
       </c>
@@ -1030,7 +1639,7 @@
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
     </row>
-    <row r="39" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" ht="20" customHeight="1" spans="1:8">
       <c r="A39" s="4">
         <v>43156</v>
       </c>
@@ -1042,7 +1651,7 @@
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
     </row>
-    <row r="40" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" ht="20" customHeight="1" spans="1:8">
       <c r="A40" s="4">
         <v>43157</v>
       </c>
@@ -1054,7 +1663,7 @@
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
     </row>
-    <row r="41" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" ht="20" customHeight="1" spans="1:8">
       <c r="A41" s="4">
         <v>43158</v>
       </c>
@@ -1066,7 +1675,7 @@
       <c r="G41" s="8"/>
       <c r="H41" s="8"/>
     </row>
-    <row r="42" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" ht="20" customHeight="1" spans="1:8">
       <c r="A42" s="4">
         <v>43159</v>
       </c>
@@ -1078,7 +1687,7 @@
       <c r="G42" s="8"/>
       <c r="H42" s="8"/>
     </row>
-    <row r="43" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" ht="20" customHeight="1" spans="1:8">
       <c r="A43" s="4">
         <v>43160</v>
       </c>
@@ -1090,7 +1699,7 @@
       <c r="G43" s="8"/>
       <c r="H43" s="8"/>
     </row>
-    <row r="44" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" ht="20" customHeight="1" spans="1:8">
       <c r="A44" s="4">
         <v>43161</v>
       </c>
@@ -1102,7 +1711,7 @@
       <c r="G44" s="8"/>
       <c r="H44" s="8"/>
     </row>
-    <row r="45" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" ht="20" customHeight="1" spans="1:8">
       <c r="A45" s="4">
         <v>43162</v>
       </c>
@@ -1114,7 +1723,7 @@
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
     </row>
-    <row r="46" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" ht="20" customHeight="1" spans="1:8">
       <c r="A46" s="4">
         <v>43163</v>
       </c>
@@ -1126,7 +1735,7 @@
       <c r="G46" s="8"/>
       <c r="H46" s="8"/>
     </row>
-    <row r="47" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" ht="20" customHeight="1" spans="1:8">
       <c r="A47" s="4">
         <v>43164</v>
       </c>
@@ -1138,7 +1747,7 @@
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
     </row>
-    <row r="48" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" ht="20" customHeight="1" spans="1:8">
       <c r="A48" s="4">
         <v>43165</v>
       </c>
@@ -1150,7 +1759,7 @@
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
     </row>
-    <row r="49" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" ht="20" customHeight="1" spans="1:8">
       <c r="A49" s="4">
         <v>43166</v>
       </c>
@@ -1162,7 +1771,7 @@
       <c r="G49" s="8"/>
       <c r="H49" s="8"/>
     </row>
-    <row r="50" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" ht="20" customHeight="1" spans="1:8">
       <c r="A50" s="4">
         <v>43167</v>
       </c>
@@ -1174,7 +1783,7 @@
       <c r="G50" s="8"/>
       <c r="H50" s="8"/>
     </row>
-    <row r="51" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" ht="20" customHeight="1" spans="1:8">
       <c r="A51" s="4">
         <v>43168</v>
       </c>
@@ -1186,7 +1795,7 @@
       <c r="G51" s="8"/>
       <c r="H51" s="8"/>
     </row>
-    <row r="52" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" ht="20" customHeight="1" spans="1:8">
       <c r="A52" s="4">
         <v>43169</v>
       </c>
@@ -1198,7 +1807,7 @@
       <c r="G52" s="8"/>
       <c r="H52" s="8"/>
     </row>
-    <row r="53" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" ht="20" customHeight="1" spans="1:8">
       <c r="A53" s="4">
         <v>43170</v>
       </c>
@@ -1210,7 +1819,7 @@
       <c r="G53" s="8"/>
       <c r="H53" s="8"/>
     </row>
-    <row r="54" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" ht="20" customHeight="1" spans="1:8">
       <c r="A54" s="4">
         <v>43171</v>
       </c>
@@ -1222,7 +1831,7 @@
       <c r="G54" s="8"/>
       <c r="H54" s="8"/>
     </row>
-    <row r="55" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" ht="20" customHeight="1" spans="1:8">
       <c r="A55" s="4">
         <v>43172</v>
       </c>
@@ -1234,7 +1843,7 @@
       <c r="G55" s="8"/>
       <c r="H55" s="8"/>
     </row>
-    <row r="56" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" ht="20" customHeight="1" spans="1:8">
       <c r="A56" s="4">
         <v>43173</v>
       </c>
@@ -1246,7 +1855,7 @@
       <c r="G56" s="8"/>
       <c r="H56" s="8"/>
     </row>
-    <row r="57" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" ht="20" customHeight="1" spans="1:8">
       <c r="A57" s="4">
         <v>43174</v>
       </c>
@@ -1258,7 +1867,7 @@
       <c r="G57" s="8"/>
       <c r="H57" s="8"/>
     </row>
-    <row r="58" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" ht="20" customHeight="1" spans="1:8">
       <c r="A58" s="4">
         <v>43175</v>
       </c>
@@ -1270,7 +1879,7 @@
       <c r="G58" s="8"/>
       <c r="H58" s="8"/>
     </row>
-    <row r="59" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" ht="20" customHeight="1" spans="1:8">
       <c r="A59" s="4">
         <v>43176</v>
       </c>
@@ -1282,7 +1891,7 @@
       <c r="G59" s="8"/>
       <c r="H59" s="8"/>
     </row>
-    <row r="60" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" ht="20" customHeight="1" spans="1:8">
       <c r="A60" s="4">
         <v>43177</v>
       </c>
@@ -1294,7 +1903,7 @@
       <c r="G60" s="8"/>
       <c r="H60" s="8"/>
     </row>
-    <row r="61" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" ht="20" customHeight="1" spans="1:8">
       <c r="A61" s="4">
         <v>43178</v>
       </c>
@@ -1306,7 +1915,7 @@
       <c r="G61" s="8"/>
       <c r="H61" s="8"/>
     </row>
-    <row r="62" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" ht="20" customHeight="1" spans="1:8">
       <c r="A62" s="4">
         <v>43179</v>
       </c>
@@ -1318,7 +1927,7 @@
       <c r="G62" s="8"/>
       <c r="H62" s="8"/>
     </row>
-    <row r="63" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" ht="20" customHeight="1" spans="1:8">
       <c r="A63" s="4">
         <v>43180</v>
       </c>
@@ -1330,7 +1939,7 @@
       <c r="G63" s="8"/>
       <c r="H63" s="8"/>
     </row>
-    <row r="64" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" ht="20" customHeight="1" spans="1:8">
       <c r="A64" s="4">
         <v>43181</v>
       </c>
@@ -1342,7 +1951,7 @@
       <c r="G64" s="8"/>
       <c r="H64" s="8"/>
     </row>
-    <row r="65" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" ht="20" customHeight="1" spans="1:8">
       <c r="A65" s="4">
         <v>43182</v>
       </c>
@@ -1354,7 +1963,7 @@
       <c r="G65" s="8"/>
       <c r="H65" s="8"/>
     </row>
-    <row r="66" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" ht="20" customHeight="1" spans="1:8">
       <c r="A66" s="4">
         <v>43183</v>
       </c>
@@ -1366,7 +1975,7 @@
       <c r="G66" s="8"/>
       <c r="H66" s="8"/>
     </row>
-    <row r="67" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" ht="20" customHeight="1" spans="1:8">
       <c r="A67" s="4">
         <v>43184</v>
       </c>
@@ -1378,7 +1987,7 @@
       <c r="G67" s="8"/>
       <c r="H67" s="8"/>
     </row>
-    <row r="68" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="68" ht="20" customHeight="1" spans="1:8">
       <c r="A68" s="4">
         <v>43185</v>
       </c>
@@ -1390,7 +1999,7 @@
       <c r="G68" s="8"/>
       <c r="H68" s="8"/>
     </row>
-    <row r="69" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="69" ht="20" customHeight="1" spans="1:8">
       <c r="A69" s="4">
         <v>43186</v>
       </c>
@@ -1402,7 +2011,7 @@
       <c r="G69" s="8"/>
       <c r="H69" s="8"/>
     </row>
-    <row r="70" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="70" ht="20" customHeight="1" spans="1:8">
       <c r="A70" s="4">
         <v>43187</v>
       </c>
@@ -1414,7 +2023,7 @@
       <c r="G70" s="8"/>
       <c r="H70" s="8"/>
     </row>
-    <row r="71" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" ht="20" customHeight="1" spans="1:8">
       <c r="A71" s="4">
         <v>43188</v>
       </c>
@@ -1426,7 +2035,7 @@
       <c r="G71" s="8"/>
       <c r="H71" s="8"/>
     </row>
-    <row r="72" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" ht="20" customHeight="1" spans="1:8">
       <c r="A72" s="4">
         <v>43189</v>
       </c>
@@ -1438,7 +2047,7 @@
       <c r="G72" s="8"/>
       <c r="H72" s="8"/>
     </row>
-    <row r="73" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="73" ht="20" customHeight="1" spans="1:8">
       <c r="A73" s="4">
         <v>43190</v>
       </c>
@@ -1450,7 +2059,7 @@
       <c r="G73" s="8"/>
       <c r="H73" s="8"/>
     </row>
-    <row r="74" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="74" ht="27" customHeight="1" spans="1:8">
       <c r="A74" s="8" t="s">
         <v>13</v>
       </c>
@@ -1463,36 +2072,42 @@
       <c r="H74" s="8"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
several days improve for me, Love but no get,thus love forever
</commit_message>
<xml_diff>
--- a/first.xlsx
+++ b/first.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13050"/>
+    <workbookView windowWidth="28695" windowHeight="12630"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27">
   <si>
     <t>Time/effective</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>车上看小说</t>
+  </si>
+  <si>
+    <t>加班</t>
+  </si>
+  <si>
+    <t>感冒了休息</t>
   </si>
   <si>
     <t>Total</t>
@@ -99,9 +105,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -112,9 +118,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -135,11 +147,55 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -159,51 +215,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -211,7 +225,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -234,7 +248,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -242,15 +256,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -307,19 +313,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -331,43 +451,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -379,19 +475,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -403,85 +487,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -510,17 +516,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -549,15 +549,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -575,20 +566,24 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -607,6 +602,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -615,10 +621,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -627,133 +633,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1160,7 +1166,7 @@
   <dimension ref="A1:P74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1380,10 +1386,10 @@
         <v>43129</v>
       </c>
       <c r="B12" s="10"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
     </row>
@@ -1391,11 +1397,13 @@
       <c r="A13" s="4">
         <v>43130</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="7"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
     </row>
@@ -1403,8 +1411,10 @@
       <c r="A14" s="4">
         <v>43131</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
+      <c r="B14" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="6"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -2121,7 +2131,7 @@
     </row>
     <row r="74" ht="27" customHeight="1" spans="1:8">
       <c r="A74" s="8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>

</xml_diff>

<commit_message>
not satisfied with these days
</commit_message>
<xml_diff>
--- a/first.xlsx
+++ b/first.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24180" windowHeight="12630"/>
+    <workbookView windowWidth="24180" windowHeight="13050"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42">
   <si>
     <t>Time/effective</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>sql join</t>
+  </si>
+  <si>
+    <t>看《和平饭店》</t>
   </si>
   <si>
     <t>Total</t>
@@ -146,10 +149,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -161,44 +164,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -207,35 +173,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -265,9 +202,66 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -289,18 +283,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -355,6 +358,60 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -367,169 +424,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -554,6 +557,63 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -585,39 +645,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -631,30 +658,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -663,145 +666,145 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="35" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1210,8 +1213,8 @@
   <sheetPr/>
   <dimension ref="A1:P74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1562,10 +1565,14 @@
       <c r="B20" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
     </row>
@@ -1573,7 +1580,9 @@
       <c r="A21" s="4">
         <v>43138</v>
       </c>
-      <c r="B21" s="8"/>
+      <c r="B21" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
@@ -2207,7 +2216,7 @@
     </row>
     <row r="74" ht="27" customHeight="1" spans="1:8">
       <c r="A74" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>

</xml_diff>

<commit_message>
spring festival and wedding
</commit_message>
<xml_diff>
--- a/first.xlsx
+++ b/first.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24180" windowHeight="13050"/>
+    <workbookView windowWidth="28695" windowHeight="13050"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47">
   <si>
     <t>Time/effective</t>
   </si>
@@ -145,6 +145,15 @@
   </si>
   <si>
     <t>sql limit 红包随机</t>
+  </si>
+  <si>
+    <t>初六</t>
+  </si>
+  <si>
+    <t>初七</t>
+  </si>
+  <si>
+    <t>初八</t>
   </si>
   <si>
     <t>Total</t>
@@ -155,10 +164,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -170,7 +179,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -185,21 +208,85 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -213,16 +300,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -242,76 +321,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="38">
     <fill>
@@ -358,19 +367,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -382,157 +475,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -576,21 +585,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -602,26 +596,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -658,6 +632,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -666,10 +675,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -678,137 +687,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -843,6 +852,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
@@ -1210,8 +1222,8 @@
   <sheetPr/>
   <dimension ref="A1:N74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1245,11 +1257,11 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="12"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="16"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="17"/>
     </row>
     <row r="2" ht="20" customHeight="1" spans="1:14">
       <c r="A2" s="4">
@@ -1597,10 +1609,10 @@
       <c r="B22" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
     </row>
@@ -1608,11 +1620,11 @@
       <c r="A23" s="4">
         <v>43140</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
     </row>
@@ -1620,11 +1632,11 @@
       <c r="A24" s="4">
         <v>43141</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
     </row>
@@ -1632,11 +1644,11 @@
       <c r="A25" s="4">
         <v>43142</v>
       </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="5"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
     </row>
@@ -1644,11 +1656,11 @@
       <c r="A26" s="4">
         <v>43143</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
     </row>
@@ -1656,11 +1668,11 @@
       <c r="A27" s="4">
         <v>43144</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
     </row>
@@ -1668,11 +1680,11 @@
       <c r="A28" s="4">
         <v>43145</v>
       </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
     </row>
@@ -1680,11 +1692,11 @@
       <c r="A29" s="4">
         <v>43146</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
     </row>
@@ -1692,11 +1704,11 @@
       <c r="A30" s="4">
         <v>43147</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
     </row>
@@ -1704,11 +1716,11 @@
       <c r="A31" s="4">
         <v>43148</v>
       </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
     </row>
@@ -1716,11 +1728,11 @@
       <c r="A32" s="4">
         <v>43149</v>
       </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
     </row>
@@ -1728,11 +1740,11 @@
       <c r="A33" s="4">
         <v>43150</v>
       </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
     </row>
@@ -1740,11 +1752,11 @@
       <c r="A34" s="4">
         <v>43151</v>
       </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
     </row>
@@ -1752,47 +1764,53 @@
       <c r="A35" s="4">
         <v>43152</v>
       </c>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="8" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1" spans="1:8">
       <c r="A36" s="4">
         <v>43153</v>
       </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="8" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1" spans="1:8">
       <c r="A37" s="4">
         <v>43154</v>
       </c>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="8" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1" spans="1:8">
       <c r="A38" s="4">
         <v>43155</v>
       </c>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
     </row>
@@ -1800,11 +1818,11 @@
       <c r="A39" s="4">
         <v>43156</v>
       </c>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
     </row>
@@ -1812,7 +1830,7 @@
       <c r="A40" s="4">
         <v>43157</v>
       </c>
-      <c r="B40" s="8"/>
+      <c r="B40" s="7"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
@@ -2218,7 +2236,7 @@
     </row>
     <row r="74" ht="27" customHeight="1" spans="1:8">
       <c r="A74" s="8" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>

</xml_diff>

<commit_message>
download pictures with python
</commit_message>
<xml_diff>
--- a/first.xlsx
+++ b/first.xlsx
@@ -164,10 +164,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -185,8 +185,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -201,9 +202,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -214,8 +215,92 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -230,97 +315,12 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="38">
     <fill>
@@ -367,181 +367,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -570,40 +570,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -624,11 +596,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -651,18 +653,16 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -675,149 +675,149 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -852,9 +852,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
@@ -1222,8 +1219,8 @@
   <sheetPr/>
   <dimension ref="A1:N74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1257,11 +1254,11 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="17"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="16"/>
     </row>
     <row r="2" ht="20" customHeight="1" spans="1:14">
       <c r="A2" s="4">
@@ -1769,7 +1766,7 @@
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
-      <c r="G35" s="12"/>
+      <c r="G35" s="8"/>
       <c r="H35" s="8" t="s">
         <v>43</v>
       </c>
@@ -1783,7 +1780,7 @@
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
-      <c r="G36" s="12"/>
+      <c r="G36" s="8"/>
       <c r="H36" s="8" t="s">
         <v>44</v>
       </c>
@@ -1797,7 +1794,7 @@
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
-      <c r="G37" s="12"/>
+      <c r="G37" s="8"/>
       <c r="H37" s="8" t="s">
         <v>45</v>
       </c>
@@ -1831,9 +1828,9 @@
         <v>43157</v>
       </c>
       <c r="B40" s="7"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="5"/>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>

</xml_diff>

<commit_message>
new serveral days day day up
</commit_message>
<xml_diff>
--- a/first.xlsx
+++ b/first.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26215"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Workspace/DongSongtao/workspace/dream_plan/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13050"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,11 +17,16 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
   <si>
     <t>Time/effective</t>
   </si>
@@ -157,19 +167,23 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>提离职</t>
+    <rPh sb="0" eb="1">
+      <t>ti</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>li'zhi</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="20">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,151 +192,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="38">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -331,7 +207,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -365,188 +241,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -569,251 +265,9 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -870,57 +324,10 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1211,25 +618,25 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.6666666666667" style="1" customWidth="1"/>
-    <col min="2" max="8" width="16.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2" max="8" width="16.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="37" customHeight="1" spans="1:14">
+    <row r="1" spans="1:14" ht="37" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1260,7 +667,7 @@
       <c r="M1" s="15"/>
       <c r="N1" s="16"/>
     </row>
-    <row r="2" ht="20" customHeight="1" spans="1:14">
+    <row r="2" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4">
         <v>43119</v>
       </c>
@@ -1289,7 +696,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" ht="20" customHeight="1" spans="1:8">
+    <row r="3" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4">
         <v>43120</v>
       </c>
@@ -1303,7 +710,7 @@
       </c>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" ht="20" customHeight="1" spans="1:8">
+    <row r="4" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4">
         <v>43121</v>
       </c>
@@ -1317,7 +724,7 @@
       </c>
       <c r="H4" s="8"/>
     </row>
-    <row r="5" ht="20" customHeight="1" spans="1:8">
+    <row r="5" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4">
         <v>43122</v>
       </c>
@@ -1331,7 +738,7 @@
       </c>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" ht="20" customHeight="1" spans="1:8">
+    <row r="6" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4">
         <v>43123</v>
       </c>
@@ -1347,7 +754,7 @@
       </c>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" ht="20" customHeight="1" spans="1:8">
+    <row r="7" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4">
         <v>43124</v>
       </c>
@@ -1371,7 +778,7 @@
       </c>
       <c r="H7" s="8"/>
     </row>
-    <row r="8" ht="20" customHeight="1" spans="1:8">
+    <row r="8" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4">
         <v>43125</v>
       </c>
@@ -1383,7 +790,7 @@
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
     </row>
-    <row r="9" ht="20" customHeight="1" spans="1:8">
+    <row r="9" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4">
         <v>43126</v>
       </c>
@@ -1399,7 +806,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" ht="20" customHeight="1" spans="1:8">
+    <row r="10" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4">
         <v>43127</v>
       </c>
@@ -1417,7 +824,7 @@
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
     </row>
-    <row r="11" ht="20" customHeight="1" spans="1:8">
+    <row r="11" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="4">
         <v>43128</v>
       </c>
@@ -1433,7 +840,7 @@
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
     </row>
-    <row r="12" ht="20" customHeight="1" spans="1:8">
+    <row r="12" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4">
         <v>43129</v>
       </c>
@@ -1445,7 +852,7 @@
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
     </row>
-    <row r="13" ht="20" customHeight="1" spans="1:8">
+    <row r="13" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4">
         <v>43130</v>
       </c>
@@ -1459,7 +866,7 @@
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
     </row>
-    <row r="14" ht="20" customHeight="1" spans="1:8">
+    <row r="14" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4">
         <v>43131</v>
       </c>
@@ -1473,7 +880,7 @@
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
     </row>
-    <row r="15" ht="20" customHeight="1" spans="1:8">
+    <row r="15" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4">
         <v>43132</v>
       </c>
@@ -1489,7 +896,7 @@
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
     </row>
-    <row r="16" ht="20" customHeight="1" spans="1:8">
+    <row r="16" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4">
         <v>43133</v>
       </c>
@@ -1505,7 +912,7 @@
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
     </row>
-    <row r="17" ht="20" customHeight="1" spans="1:8">
+    <row r="17" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4">
         <v>43134</v>
       </c>
@@ -1527,7 +934,7 @@
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
     </row>
-    <row r="18" ht="20" customHeight="1" spans="1:8">
+    <row r="18" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="4">
         <v>43135</v>
       </c>
@@ -1545,7 +952,7 @@
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
     </row>
-    <row r="19" ht="20" customHeight="1" spans="1:8">
+    <row r="19" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="4">
         <v>43136</v>
       </c>
@@ -1563,7 +970,7 @@
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
     </row>
-    <row r="20" ht="20" customHeight="1" spans="1:8">
+    <row r="20" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="4">
         <v>43137</v>
       </c>
@@ -1581,7 +988,7 @@
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
     </row>
-    <row r="21" ht="20" customHeight="1" spans="1:8">
+    <row r="21" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="4">
         <v>43138</v>
       </c>
@@ -1599,7 +1006,7 @@
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
     </row>
-    <row r="22" ht="20" customHeight="1" spans="1:8">
+    <row r="22" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="4">
         <v>43139</v>
       </c>
@@ -1613,7 +1020,7 @@
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
     </row>
-    <row r="23" ht="20" customHeight="1" spans="1:8">
+    <row r="23" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="4">
         <v>43140</v>
       </c>
@@ -1625,7 +1032,7 @@
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
     </row>
-    <row r="24" ht="20" customHeight="1" spans="1:8">
+    <row r="24" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="4">
         <v>43141</v>
       </c>
@@ -1637,7 +1044,7 @@
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
     </row>
-    <row r="25" ht="20" customHeight="1" spans="1:8">
+    <row r="25" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="4">
         <v>43142</v>
       </c>
@@ -1649,7 +1056,7 @@
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
     </row>
-    <row r="26" ht="20" customHeight="1" spans="1:8">
+    <row r="26" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="4">
         <v>43143</v>
       </c>
@@ -1661,7 +1068,7 @@
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
     </row>
-    <row r="27" ht="20" customHeight="1" spans="1:8">
+    <row r="27" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="4">
         <v>43144</v>
       </c>
@@ -1673,7 +1080,7 @@
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
     </row>
-    <row r="28" ht="20" customHeight="1" spans="1:8">
+    <row r="28" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="4">
         <v>43145</v>
       </c>
@@ -1685,7 +1092,7 @@
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
     </row>
-    <row r="29" ht="20" customHeight="1" spans="1:8">
+    <row r="29" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="4">
         <v>43146</v>
       </c>
@@ -1697,7 +1104,7 @@
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
     </row>
-    <row r="30" ht="20" customHeight="1" spans="1:8">
+    <row r="30" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="4">
         <v>43147</v>
       </c>
@@ -1709,7 +1116,7 @@
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
     </row>
-    <row r="31" ht="20" customHeight="1" spans="1:8">
+    <row r="31" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="4">
         <v>43148</v>
       </c>
@@ -1721,7 +1128,7 @@
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
     </row>
-    <row r="32" ht="20" customHeight="1" spans="1:8">
+    <row r="32" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="4">
         <v>43149</v>
       </c>
@@ -1733,7 +1140,7 @@
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
     </row>
-    <row r="33" ht="20" customHeight="1" spans="1:8">
+    <row r="33" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="4">
         <v>43150</v>
       </c>
@@ -1745,7 +1152,7 @@
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
     </row>
-    <row r="34" ht="20" customHeight="1" spans="1:8">
+    <row r="34" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="4">
         <v>43151</v>
       </c>
@@ -1757,7 +1164,7 @@
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
     </row>
-    <row r="35" ht="20" customHeight="1" spans="1:8">
+    <row r="35" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="4">
         <v>43152</v>
       </c>
@@ -1771,7 +1178,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" ht="20" customHeight="1" spans="1:8">
+    <row r="36" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="4">
         <v>43153</v>
       </c>
@@ -1785,7 +1192,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" ht="20" customHeight="1" spans="1:8">
+    <row r="37" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="4">
         <v>43154</v>
       </c>
@@ -1799,7 +1206,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" ht="20" customHeight="1" spans="1:8">
+    <row r="38" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="4">
         <v>43155</v>
       </c>
@@ -1811,7 +1218,7 @@
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
     </row>
-    <row r="39" ht="20" customHeight="1" spans="1:8">
+    <row r="39" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="4">
         <v>43156</v>
       </c>
@@ -1823,7 +1230,7 @@
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
     </row>
-    <row r="40" ht="20" customHeight="1" spans="1:8">
+    <row r="40" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="4">
         <v>43157</v>
       </c>
@@ -1835,67 +1242,69 @@
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
     </row>
-    <row r="41" ht="20" customHeight="1" spans="1:8">
+    <row r="41" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="4">
         <v>43158</v>
       </c>
       <c r="B41" s="10"/>
       <c r="C41" s="9"/>
       <c r="D41" s="7"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
       <c r="G41" s="8"/>
       <c r="H41" s="8"/>
     </row>
-    <row r="42" ht="20" customHeight="1" spans="1:8">
+    <row r="42" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="4">
         <v>43159</v>
       </c>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
       <c r="G42" s="8"/>
       <c r="H42" s="8"/>
     </row>
-    <row r="43" ht="20" customHeight="1" spans="1:8">
+    <row r="43" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="4">
         <v>43160</v>
       </c>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F43" s="7"/>
       <c r="G43" s="8"/>
       <c r="H43" s="8"/>
     </row>
-    <row r="44" ht="20" customHeight="1" spans="1:8">
+    <row r="44" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="4">
         <v>43161</v>
       </c>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
       <c r="G44" s="8"/>
       <c r="H44" s="8"/>
     </row>
-    <row r="45" ht="20" customHeight="1" spans="1:8">
+    <row r="45" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="4">
         <v>43162</v>
       </c>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
     </row>
-    <row r="46" ht="20" customHeight="1" spans="1:8">
+    <row r="46" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="4">
         <v>43163</v>
       </c>
@@ -1907,7 +1316,7 @@
       <c r="G46" s="8"/>
       <c r="H46" s="8"/>
     </row>
-    <row r="47" ht="20" customHeight="1" spans="1:8">
+    <row r="47" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="4">
         <v>43164</v>
       </c>
@@ -1919,7 +1328,7 @@
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
     </row>
-    <row r="48" ht="20" customHeight="1" spans="1:8">
+    <row r="48" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="4">
         <v>43165</v>
       </c>
@@ -1931,7 +1340,7 @@
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
     </row>
-    <row r="49" ht="20" customHeight="1" spans="1:8">
+    <row r="49" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="4">
         <v>43166</v>
       </c>
@@ -1943,7 +1352,7 @@
       <c r="G49" s="8"/>
       <c r="H49" s="8"/>
     </row>
-    <row r="50" ht="20" customHeight="1" spans="1:8">
+    <row r="50" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="4">
         <v>43167</v>
       </c>
@@ -1955,7 +1364,7 @@
       <c r="G50" s="8"/>
       <c r="H50" s="8"/>
     </row>
-    <row r="51" ht="20" customHeight="1" spans="1:8">
+    <row r="51" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="4">
         <v>43168</v>
       </c>
@@ -1967,7 +1376,7 @@
       <c r="G51" s="8"/>
       <c r="H51" s="8"/>
     </row>
-    <row r="52" ht="20" customHeight="1" spans="1:8">
+    <row r="52" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="4">
         <v>43169</v>
       </c>
@@ -1979,7 +1388,7 @@
       <c r="G52" s="8"/>
       <c r="H52" s="8"/>
     </row>
-    <row r="53" ht="20" customHeight="1" spans="1:8">
+    <row r="53" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="4">
         <v>43170</v>
       </c>
@@ -1991,7 +1400,7 @@
       <c r="G53" s="8"/>
       <c r="H53" s="8"/>
     </row>
-    <row r="54" ht="20" customHeight="1" spans="1:8">
+    <row r="54" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="4">
         <v>43171</v>
       </c>
@@ -2003,7 +1412,7 @@
       <c r="G54" s="8"/>
       <c r="H54" s="8"/>
     </row>
-    <row r="55" ht="20" customHeight="1" spans="1:8">
+    <row r="55" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="4">
         <v>43172</v>
       </c>
@@ -2015,7 +1424,7 @@
       <c r="G55" s="8"/>
       <c r="H55" s="8"/>
     </row>
-    <row r="56" ht="20" customHeight="1" spans="1:8">
+    <row r="56" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="4">
         <v>43173</v>
       </c>
@@ -2027,7 +1436,7 @@
       <c r="G56" s="8"/>
       <c r="H56" s="8"/>
     </row>
-    <row r="57" ht="20" customHeight="1" spans="1:8">
+    <row r="57" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="4">
         <v>43174</v>
       </c>
@@ -2039,7 +1448,7 @@
       <c r="G57" s="8"/>
       <c r="H57" s="8"/>
     </row>
-    <row r="58" ht="20" customHeight="1" spans="1:8">
+    <row r="58" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="4">
         <v>43175</v>
       </c>
@@ -2051,7 +1460,7 @@
       <c r="G58" s="8"/>
       <c r="H58" s="8"/>
     </row>
-    <row r="59" ht="20" customHeight="1" spans="1:8">
+    <row r="59" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="4">
         <v>43176</v>
       </c>
@@ -2063,7 +1472,7 @@
       <c r="G59" s="8"/>
       <c r="H59" s="8"/>
     </row>
-    <row r="60" ht="20" customHeight="1" spans="1:8">
+    <row r="60" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="4">
         <v>43177</v>
       </c>
@@ -2075,7 +1484,7 @@
       <c r="G60" s="8"/>
       <c r="H60" s="8"/>
     </row>
-    <row r="61" ht="20" customHeight="1" spans="1:8">
+    <row r="61" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="4">
         <v>43178</v>
       </c>
@@ -2087,7 +1496,7 @@
       <c r="G61" s="8"/>
       <c r="H61" s="8"/>
     </row>
-    <row r="62" ht="20" customHeight="1" spans="1:8">
+    <row r="62" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="4">
         <v>43179</v>
       </c>
@@ -2099,7 +1508,7 @@
       <c r="G62" s="8"/>
       <c r="H62" s="8"/>
     </row>
-    <row r="63" ht="20" customHeight="1" spans="1:8">
+    <row r="63" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="4">
         <v>43180</v>
       </c>
@@ -2111,7 +1520,7 @@
       <c r="G63" s="8"/>
       <c r="H63" s="8"/>
     </row>
-    <row r="64" ht="20" customHeight="1" spans="1:8">
+    <row r="64" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="4">
         <v>43181</v>
       </c>
@@ -2123,7 +1532,7 @@
       <c r="G64" s="8"/>
       <c r="H64" s="8"/>
     </row>
-    <row r="65" ht="20" customHeight="1" spans="1:8">
+    <row r="65" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="4">
         <v>43182</v>
       </c>
@@ -2135,7 +1544,7 @@
       <c r="G65" s="8"/>
       <c r="H65" s="8"/>
     </row>
-    <row r="66" ht="20" customHeight="1" spans="1:8">
+    <row r="66" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="4">
         <v>43183</v>
       </c>
@@ -2147,7 +1556,7 @@
       <c r="G66" s="8"/>
       <c r="H66" s="8"/>
     </row>
-    <row r="67" ht="20" customHeight="1" spans="1:8">
+    <row r="67" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="4">
         <v>43184</v>
       </c>
@@ -2159,7 +1568,7 @@
       <c r="G67" s="8"/>
       <c r="H67" s="8"/>
     </row>
-    <row r="68" ht="20" customHeight="1" spans="1:8">
+    <row r="68" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="4">
         <v>43185</v>
       </c>
@@ -2171,7 +1580,7 @@
       <c r="G68" s="8"/>
       <c r="H68" s="8"/>
     </row>
-    <row r="69" ht="20" customHeight="1" spans="1:8">
+    <row r="69" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="4">
         <v>43186</v>
       </c>
@@ -2183,7 +1592,7 @@
       <c r="G69" s="8"/>
       <c r="H69" s="8"/>
     </row>
-    <row r="70" ht="20" customHeight="1" spans="1:8">
+    <row r="70" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="4">
         <v>43187</v>
       </c>
@@ -2195,7 +1604,7 @@
       <c r="G70" s="8"/>
       <c r="H70" s="8"/>
     </row>
-    <row r="71" ht="20" customHeight="1" spans="1:8">
+    <row r="71" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="4">
         <v>43188</v>
       </c>
@@ -2207,7 +1616,7 @@
       <c r="G71" s="8"/>
       <c r="H71" s="8"/>
     </row>
-    <row r="72" ht="20" customHeight="1" spans="1:8">
+    <row r="72" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="4">
         <v>43189</v>
       </c>
@@ -2219,7 +1628,7 @@
       <c r="G72" s="8"/>
       <c r="H72" s="8"/>
     </row>
-    <row r="73" ht="20" customHeight="1" spans="1:8">
+    <row r="73" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="4">
         <v>43190</v>
       </c>
@@ -2231,7 +1640,7 @@
       <c r="G73" s="8"/>
       <c r="H73" s="8"/>
     </row>
-    <row r="74" ht="27" customHeight="1" spans="1:8">
+    <row r="74" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="8" t="s">
         <v>46</v>
       </c>
@@ -2244,42 +1653,36 @@
       <c r="H74" s="8"/>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <sheetData/>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <sheetData/>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new serveral perfect days, keep your step of learning
</commit_message>
<xml_diff>
--- a/first.xlsx
+++ b/first.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
   <si>
     <t>Time/effective</t>
   </si>
@@ -175,6 +175,22 @@
     </rPh>
     <rPh sb="1" eb="2">
       <t>li'zhi</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>滨生来杭州</t>
+    <rPh sb="0" eb="1">
+      <t>bin'sheng</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>sheng</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>lai</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>hang'zhou</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -626,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1300,7 +1316,7 @@
       <c r="C45" s="9"/>
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
-      <c r="F45" s="8"/>
+      <c r="F45" s="10"/>
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
     </row>
@@ -1308,11 +1324,11 @@
       <c r="A46" s="4">
         <v>43163</v>
       </c>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="9"/>
       <c r="G46" s="8"/>
       <c r="H46" s="8"/>
     </row>
@@ -1320,11 +1336,11 @@
       <c r="A47" s="4">
         <v>43164</v>
       </c>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="8"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="7"/>
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
     </row>
@@ -1332,10 +1348,12 @@
       <c r="A48" s="4">
         <v>43165</v>
       </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9" t="s">
+        <v>48</v>
+      </c>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>

</xml_diff>

<commit_message>
the last ten days are wasted, my god, you silly boy
</commit_message>
<xml_diff>
--- a/first.xlsx
+++ b/first.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26215"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Workspace/DongSongtao/workspace/dream_plan/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="640" windowWidth="25600" windowHeight="13060"/>
+    <workbookView windowWidth="28695" windowHeight="13050"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,16 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60">
   <si>
     <t>Time/effective</t>
   </si>
@@ -166,40 +156,59 @@
     <t>初八</t>
   </si>
   <si>
+    <t>提离职</t>
+  </si>
+  <si>
+    <t>滨生来杭州</t>
+  </si>
+  <si>
+    <t>追书贵族纹章</t>
+  </si>
+  <si>
+    <t>白夜追凶</t>
+  </si>
+  <si>
+    <t>口袋3终极试炼</t>
+  </si>
+  <si>
+    <t>和滨生聊天</t>
+  </si>
+  <si>
+    <t>看lua</t>
+  </si>
+  <si>
+    <t>公司加班</t>
+  </si>
+  <si>
+    <t>lua正态分布随机</t>
+  </si>
+  <si>
+    <t>周日</t>
+  </si>
+  <si>
+    <t>玩下一个英雄王</t>
+  </si>
+  <si>
+    <t>睡的还行</t>
+  </si>
+  <si>
+    <t>8点46才起来</t>
+  </si>
+  <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>提离职</t>
-    <rPh sb="0" eb="1">
-      <t>ti</t>
-    </rPh>
-    <rPh sb="1" eb="2">
-      <t>li'zhi</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>滨生来杭州</t>
-    <rPh sb="0" eb="1">
-      <t>bin'sheng</t>
-    </rPh>
-    <rPh sb="1" eb="2">
-      <t>sheng</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>lai</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>hang'zhou</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,13 +217,151 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -223,7 +370,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -257,8 +404,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -281,9 +614,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -340,10 +915,57 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -634,25 +1256,25 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:N74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2" max="8" width="16.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6666666666667" style="1" customWidth="1"/>
+    <col min="2" max="8" width="16.6666666666667" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="37" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" ht="37" customHeight="1" spans="1:14">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -683,7 +1305,7 @@
       <c r="M1" s="15"/>
       <c r="N1" s="16"/>
     </row>
-    <row r="2" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" ht="20" customHeight="1" spans="1:14">
       <c r="A2" s="4">
         <v>43119</v>
       </c>
@@ -712,7 +1334,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" ht="20" customHeight="1" spans="1:8">
       <c r="A3" s="4">
         <v>43120</v>
       </c>
@@ -726,7 +1348,7 @@
       </c>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" ht="20" customHeight="1" spans="1:8">
       <c r="A4" s="4">
         <v>43121</v>
       </c>
@@ -740,7 +1362,7 @@
       </c>
       <c r="H4" s="8"/>
     </row>
-    <row r="5" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" ht="20" customHeight="1" spans="1:8">
       <c r="A5" s="4">
         <v>43122</v>
       </c>
@@ -754,7 +1376,7 @@
       </c>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" ht="20" customHeight="1" spans="1:8">
       <c r="A6" s="4">
         <v>43123</v>
       </c>
@@ -770,7 +1392,7 @@
       </c>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" ht="20" customHeight="1" spans="1:8">
       <c r="A7" s="4">
         <v>43124</v>
       </c>
@@ -794,7 +1416,7 @@
       </c>
       <c r="H7" s="8"/>
     </row>
-    <row r="8" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" ht="20" customHeight="1" spans="1:8">
       <c r="A8" s="4">
         <v>43125</v>
       </c>
@@ -806,7 +1428,7 @@
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
     </row>
-    <row r="9" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" ht="20" customHeight="1" spans="1:8">
       <c r="A9" s="4">
         <v>43126</v>
       </c>
@@ -822,7 +1444,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" ht="20" customHeight="1" spans="1:8">
       <c r="A10" s="4">
         <v>43127</v>
       </c>
@@ -840,7 +1462,7 @@
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
     </row>
-    <row r="11" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" ht="20" customHeight="1" spans="1:8">
       <c r="A11" s="4">
         <v>43128</v>
       </c>
@@ -856,7 +1478,7 @@
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
     </row>
-    <row r="12" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" ht="20" customHeight="1" spans="1:8">
       <c r="A12" s="4">
         <v>43129</v>
       </c>
@@ -868,7 +1490,7 @@
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
     </row>
-    <row r="13" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" ht="20" customHeight="1" spans="1:8">
       <c r="A13" s="4">
         <v>43130</v>
       </c>
@@ -882,7 +1504,7 @@
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
     </row>
-    <row r="14" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" ht="20" customHeight="1" spans="1:8">
       <c r="A14" s="4">
         <v>43131</v>
       </c>
@@ -896,7 +1518,7 @@
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
     </row>
-    <row r="15" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" ht="20" customHeight="1" spans="1:8">
       <c r="A15" s="4">
         <v>43132</v>
       </c>
@@ -912,7 +1534,7 @@
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
     </row>
-    <row r="16" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" ht="20" customHeight="1" spans="1:8">
       <c r="A16" s="4">
         <v>43133</v>
       </c>
@@ -928,7 +1550,7 @@
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
     </row>
-    <row r="17" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" ht="20" customHeight="1" spans="1:8">
       <c r="A17" s="4">
         <v>43134</v>
       </c>
@@ -950,7 +1572,7 @@
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
     </row>
-    <row r="18" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" ht="20" customHeight="1" spans="1:8">
       <c r="A18" s="4">
         <v>43135</v>
       </c>
@@ -968,7 +1590,7 @@
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
     </row>
-    <row r="19" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" ht="20" customHeight="1" spans="1:8">
       <c r="A19" s="4">
         <v>43136</v>
       </c>
@@ -986,7 +1608,7 @@
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
     </row>
-    <row r="20" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" ht="20" customHeight="1" spans="1:8">
       <c r="A20" s="4">
         <v>43137</v>
       </c>
@@ -1004,7 +1626,7 @@
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
     </row>
-    <row r="21" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" ht="20" customHeight="1" spans="1:8">
       <c r="A21" s="4">
         <v>43138</v>
       </c>
@@ -1022,7 +1644,7 @@
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
     </row>
-    <row r="22" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" ht="20" customHeight="1" spans="1:8">
       <c r="A22" s="4">
         <v>43139</v>
       </c>
@@ -1036,7 +1658,7 @@
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
     </row>
-    <row r="23" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" ht="20" customHeight="1" spans="1:8">
       <c r="A23" s="4">
         <v>43140</v>
       </c>
@@ -1048,7 +1670,7 @@
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
     </row>
-    <row r="24" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" ht="20" customHeight="1" spans="1:8">
       <c r="A24" s="4">
         <v>43141</v>
       </c>
@@ -1060,7 +1682,7 @@
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
     </row>
-    <row r="25" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" ht="20" customHeight="1" spans="1:8">
       <c r="A25" s="4">
         <v>43142</v>
       </c>
@@ -1072,7 +1694,7 @@
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
     </row>
-    <row r="26" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" ht="20" customHeight="1" spans="1:8">
       <c r="A26" s="4">
         <v>43143</v>
       </c>
@@ -1084,7 +1706,7 @@
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
     </row>
-    <row r="27" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" ht="20" customHeight="1" spans="1:8">
       <c r="A27" s="4">
         <v>43144</v>
       </c>
@@ -1096,7 +1718,7 @@
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
     </row>
-    <row r="28" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" ht="20" customHeight="1" spans="1:8">
       <c r="A28" s="4">
         <v>43145</v>
       </c>
@@ -1108,7 +1730,7 @@
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
     </row>
-    <row r="29" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" ht="20" customHeight="1" spans="1:8">
       <c r="A29" s="4">
         <v>43146</v>
       </c>
@@ -1120,7 +1742,7 @@
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
     </row>
-    <row r="30" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" ht="20" customHeight="1" spans="1:8">
       <c r="A30" s="4">
         <v>43147</v>
       </c>
@@ -1132,7 +1754,7 @@
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
     </row>
-    <row r="31" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" ht="20" customHeight="1" spans="1:8">
       <c r="A31" s="4">
         <v>43148</v>
       </c>
@@ -1144,7 +1766,7 @@
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
     </row>
-    <row r="32" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" ht="20" customHeight="1" spans="1:8">
       <c r="A32" s="4">
         <v>43149</v>
       </c>
@@ -1156,7 +1778,7 @@
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
     </row>
-    <row r="33" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" ht="20" customHeight="1" spans="1:8">
       <c r="A33" s="4">
         <v>43150</v>
       </c>
@@ -1168,7 +1790,7 @@
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
     </row>
-    <row r="34" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" ht="20" customHeight="1" spans="1:8">
       <c r="A34" s="4">
         <v>43151</v>
       </c>
@@ -1180,7 +1802,7 @@
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
     </row>
-    <row r="35" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" ht="20" customHeight="1" spans="1:8">
       <c r="A35" s="4">
         <v>43152</v>
       </c>
@@ -1194,7 +1816,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" ht="20" customHeight="1" spans="1:8">
       <c r="A36" s="4">
         <v>43153</v>
       </c>
@@ -1208,7 +1830,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" ht="20" customHeight="1" spans="1:8">
       <c r="A37" s="4">
         <v>43154</v>
       </c>
@@ -1222,7 +1844,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" ht="20" customHeight="1" spans="1:8">
       <c r="A38" s="4">
         <v>43155</v>
       </c>
@@ -1234,7 +1856,7 @@
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
     </row>
-    <row r="39" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" ht="20" customHeight="1" spans="1:8">
       <c r="A39" s="4">
         <v>43156</v>
       </c>
@@ -1246,7 +1868,7 @@
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
     </row>
-    <row r="40" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" ht="20" customHeight="1" spans="1:8">
       <c r="A40" s="4">
         <v>43157</v>
       </c>
@@ -1258,7 +1880,7 @@
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
     </row>
-    <row r="41" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" ht="20" customHeight="1" spans="1:8">
       <c r="A41" s="4">
         <v>43158</v>
       </c>
@@ -1270,7 +1892,7 @@
       <c r="G41" s="8"/>
       <c r="H41" s="8"/>
     </row>
-    <row r="42" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" ht="20" customHeight="1" spans="1:8">
       <c r="A42" s="4">
         <v>43159</v>
       </c>
@@ -1282,7 +1904,7 @@
       <c r="G42" s="8"/>
       <c r="H42" s="8"/>
     </row>
-    <row r="43" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" ht="20" customHeight="1" spans="1:8">
       <c r="A43" s="4">
         <v>43160</v>
       </c>
@@ -1290,13 +1912,13 @@
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="8"/>
       <c r="H43" s="8"/>
     </row>
-    <row r="44" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" ht="20" customHeight="1" spans="1:8">
       <c r="A44" s="4">
         <v>43161</v>
       </c>
@@ -1308,7 +1930,7 @@
       <c r="G44" s="8"/>
       <c r="H44" s="8"/>
     </row>
-    <row r="45" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" ht="20" customHeight="1" spans="1:8">
       <c r="A45" s="4">
         <v>43162</v>
       </c>
@@ -1320,7 +1942,7 @@
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
     </row>
-    <row r="46" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" ht="20" customHeight="1" spans="1:8">
       <c r="A46" s="4">
         <v>43163</v>
       </c>
@@ -1332,7 +1954,7 @@
       <c r="G46" s="8"/>
       <c r="H46" s="8"/>
     </row>
-    <row r="47" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" ht="20" customHeight="1" spans="1:8">
       <c r="A47" s="4">
         <v>43164</v>
       </c>
@@ -1344,7 +1966,7 @@
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
     </row>
-    <row r="48" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" ht="20" customHeight="1" spans="1:8">
       <c r="A48" s="4">
         <v>43165</v>
       </c>
@@ -1352,13 +1974,13 @@
       <c r="C48" s="9"/>
       <c r="D48" s="9"/>
       <c r="E48" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F48" s="7"/>
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
     </row>
-    <row r="49" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" ht="20" customHeight="1" spans="1:8">
       <c r="A49" s="4">
         <v>43166</v>
       </c>
@@ -1370,7 +1992,7 @@
       <c r="G49" s="8"/>
       <c r="H49" s="8"/>
     </row>
-    <row r="50" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" ht="20" customHeight="1" spans="1:8">
       <c r="A50" s="4">
         <v>43167</v>
       </c>
@@ -1382,131 +2004,187 @@
       <c r="G50" s="8"/>
       <c r="H50" s="8"/>
     </row>
-    <row r="51" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" ht="20" customHeight="1" spans="1:8">
       <c r="A51" s="4">
         <v>43168</v>
       </c>
       <c r="B51" s="9"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
       <c r="G51" s="8"/>
       <c r="H51" s="8"/>
     </row>
-    <row r="52" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" ht="20" customHeight="1" spans="1:8">
       <c r="A52" s="4">
         <v>43169</v>
       </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="8"/>
-      <c r="F52" s="8"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F52" s="11"/>
       <c r="G52" s="8"/>
       <c r="H52" s="8"/>
     </row>
-    <row r="53" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" ht="20" customHeight="1" spans="1:8">
       <c r="A53" s="4">
         <v>43170</v>
       </c>
-      <c r="B53" s="8"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="8"/>
-      <c r="F53" s="8"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="G53" s="8"/>
       <c r="H53" s="8"/>
     </row>
-    <row r="54" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" ht="20" customHeight="1" spans="1:8">
       <c r="A54" s="4">
         <v>43171</v>
       </c>
-      <c r="B54" s="8"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
-      <c r="F54" s="8"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F54" s="7"/>
       <c r="G54" s="8"/>
       <c r="H54" s="8"/>
     </row>
-    <row r="55" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" ht="20" customHeight="1" spans="1:8">
       <c r="A55" s="4">
         <v>43172</v>
       </c>
-      <c r="B55" s="8"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="8"/>
-      <c r="F55" s="8"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E55" s="9"/>
+      <c r="F55" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="G55" s="8"/>
       <c r="H55" s="8"/>
     </row>
-    <row r="56" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" ht="20" customHeight="1" spans="1:8">
       <c r="A56" s="4">
         <v>43173</v>
       </c>
-      <c r="B56" s="8"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
-      <c r="F56" s="8"/>
+      <c r="B56" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E56" s="9"/>
+      <c r="F56" s="7"/>
       <c r="G56" s="8"/>
       <c r="H56" s="8"/>
     </row>
-    <row r="57" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" ht="20" customHeight="1" spans="1:8">
       <c r="A57" s="4">
         <v>43174</v>
       </c>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
-      <c r="F57" s="8"/>
+      <c r="B57" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F57" s="7"/>
       <c r="G57" s="8"/>
       <c r="H57" s="8"/>
     </row>
-    <row r="58" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" ht="20" customHeight="1" spans="1:8">
       <c r="A58" s="4">
         <v>43175</v>
       </c>
-      <c r="B58" s="8"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
-      <c r="F58" s="8"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
       <c r="G58" s="8"/>
       <c r="H58" s="8"/>
     </row>
-    <row r="59" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" ht="20" customHeight="1" spans="1:8">
       <c r="A59" s="4">
         <v>43176</v>
       </c>
-      <c r="B59" s="8"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="8"/>
-      <c r="E59" s="8"/>
-      <c r="F59" s="8"/>
-      <c r="G59" s="8"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F59" s="7"/>
+      <c r="G59" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="H59" s="8"/>
     </row>
-    <row r="60" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" ht="20" customHeight="1" spans="1:8">
       <c r="A60" s="4">
         <v>43177</v>
       </c>
-      <c r="B60" s="8"/>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="8"/>
-      <c r="F60" s="8"/>
+      <c r="B60" s="6"/>
+      <c r="C60" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F60" s="9" t="s">
+        <v>57</v>
+      </c>
       <c r="G60" s="8"/>
       <c r="H60" s="8"/>
     </row>
-    <row r="61" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" ht="20" customHeight="1" spans="1:8">
       <c r="A61" s="4">
         <v>43178</v>
       </c>
-      <c r="B61" s="8"/>
+      <c r="B61" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
       <c r="E61" s="8"/>
@@ -1514,7 +2192,7 @@
       <c r="G61" s="8"/>
       <c r="H61" s="8"/>
     </row>
-    <row r="62" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" ht="20" customHeight="1" spans="1:8">
       <c r="A62" s="4">
         <v>43179</v>
       </c>
@@ -1526,7 +2204,7 @@
       <c r="G62" s="8"/>
       <c r="H62" s="8"/>
     </row>
-    <row r="63" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" ht="20" customHeight="1" spans="1:8">
       <c r="A63" s="4">
         <v>43180</v>
       </c>
@@ -1538,7 +2216,7 @@
       <c r="G63" s="8"/>
       <c r="H63" s="8"/>
     </row>
-    <row r="64" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" ht="20" customHeight="1" spans="1:8">
       <c r="A64" s="4">
         <v>43181</v>
       </c>
@@ -1550,7 +2228,7 @@
       <c r="G64" s="8"/>
       <c r="H64" s="8"/>
     </row>
-    <row r="65" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" ht="20" customHeight="1" spans="1:8">
       <c r="A65" s="4">
         <v>43182</v>
       </c>
@@ -1562,7 +2240,7 @@
       <c r="G65" s="8"/>
       <c r="H65" s="8"/>
     </row>
-    <row r="66" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" ht="20" customHeight="1" spans="1:8">
       <c r="A66" s="4">
         <v>43183</v>
       </c>
@@ -1574,7 +2252,7 @@
       <c r="G66" s="8"/>
       <c r="H66" s="8"/>
     </row>
-    <row r="67" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" ht="20" customHeight="1" spans="1:8">
       <c r="A67" s="4">
         <v>43184</v>
       </c>
@@ -1586,7 +2264,7 @@
       <c r="G67" s="8"/>
       <c r="H67" s="8"/>
     </row>
-    <row r="68" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="68" ht="20" customHeight="1" spans="1:8">
       <c r="A68" s="4">
         <v>43185</v>
       </c>
@@ -1598,7 +2276,7 @@
       <c r="G68" s="8"/>
       <c r="H68" s="8"/>
     </row>
-    <row r="69" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="69" ht="20" customHeight="1" spans="1:8">
       <c r="A69" s="4">
         <v>43186</v>
       </c>
@@ -1610,7 +2288,7 @@
       <c r="G69" s="8"/>
       <c r="H69" s="8"/>
     </row>
-    <row r="70" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="70" ht="20" customHeight="1" spans="1:8">
       <c r="A70" s="4">
         <v>43187</v>
       </c>
@@ -1622,7 +2300,7 @@
       <c r="G70" s="8"/>
       <c r="H70" s="8"/>
     </row>
-    <row r="71" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" ht="20" customHeight="1" spans="1:8">
       <c r="A71" s="4">
         <v>43188</v>
       </c>
@@ -1634,7 +2312,7 @@
       <c r="G71" s="8"/>
       <c r="H71" s="8"/>
     </row>
-    <row r="72" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" ht="20" customHeight="1" spans="1:8">
       <c r="A72" s="4">
         <v>43189</v>
       </c>
@@ -1646,7 +2324,7 @@
       <c r="G72" s="8"/>
       <c r="H72" s="8"/>
     </row>
-    <row r="73" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="73" ht="20" customHeight="1" spans="1:8">
       <c r="A73" s="4">
         <v>43190</v>
       </c>
@@ -1658,9 +2336,9 @@
       <c r="G73" s="8"/>
       <c r="H73" s="8"/>
     </row>
-    <row r="74" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="74" ht="27" customHeight="1" spans="1:8">
       <c r="A74" s="8" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>
@@ -1671,36 +2349,42 @@
       <c r="H74" s="8"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>